<commit_message>
perbaiki logika bayar di routeTransaction.py bagian insert detailTransaksi
</commit_message>
<xml_diff>
--- a/datapenjualan_bushub.xlsx
+++ b/datapenjualan_bushub.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,32 +541,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-11-10 18:29:09.052643+07:00</t>
+          <t>2024-11-25 18:03:54.803392+07:00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>user1@gmail.com</t>
+          <t>user2@gmail.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ST001</t>
+          <t>KSR_01</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>CANCELLED</t>
+          <t>COMPLETED</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>500000.0</t>
+          <t>2280000.0</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>cash</t>
+          <t>transfer</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -584,11 +584,7 @@
           <t>PTKSKW</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Paket Wisata Singkawang</t>
-        </is>
-      </c>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -598,17 +594,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-11-10 18:37:37.082473+07:00</t>
+          <t>2024-11-25 18:05:21.359478+07:00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>user1@gmail.com</t>
+          <t>user2@gmail.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ST001</t>
+          <t>KSR_01</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -618,7 +614,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>1500000.0</t>
+          <t>500000.0</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -628,12 +624,12 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2024-12-02</t>
+          <t>2024-11-25</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2024-12-04</t>
+          <t>2024-11-26</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -643,39 +639,39 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Paket Wisata Ketapang</t>
+          <t>Paket Wisata Singkawang</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>A0006</t>
+          <t>A0003</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-11-10 18:47:34.299202+07:00</t>
+          <t>2024-11-25 18:03:54.803392+07:00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>user1@gmail.com</t>
+          <t>user2@gmail.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ST001</t>
+          <t>KSR_01</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CANCELLED</t>
+          <t>COMPLETED</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1520000.0</t>
+          <t>2280000.0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -685,12 +681,12 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2024-11-12</t>
+          <t>2024-11-25</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2024-11-21</t>
+          <t>2024-11-28</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -703,22 +699,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>A0007</t>
+          <t>A0004</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-11-10 18:48:48.197088+07:00</t>
+          <t>2024-11-25 18:05:21.359478+07:00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>user1@gmail.com</t>
+          <t>user2@gmail.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ST001</t>
+          <t>KSR_01</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -754,63 +750,6 @@
       <c r="K8" t="inlineStr">
         <is>
           <t>Paket Wisata Singkawang</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>A0010</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2024-11-16 20:01:30.533485+07:00</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>user1@gmail.com</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>ST001</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>CANCELLED</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>1500000.0</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>transfer</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>2024-12-02</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>2024-12-04</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>PTKSKW</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Paket Wisata Ketapang</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Perbaiki logika /checkout di routeTransaction.py lalu routeAdmin.py bagian /dataTrans/{id}
</commit_message>
<xml_diff>
--- a/datapenjualan_bushub.xlsx
+++ b/datapenjualan_bushub.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,12 +536,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>A0003</t>
+          <t>A0001</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-11-25 18:03:54.803392+07:00</t>
+          <t>2024-11-27 03:21:34.900792+07:00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>KSR_01</t>
+          <t>ADM_01</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -561,22 +561,22 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2280000.0</t>
+          <t>1500000.0</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>transfer</t>
+          <t>cash</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2024-11-30</t>
+          <t>2024-12-02</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2024-12-04</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -584,27 +584,31 @@
           <t>PTKSKW</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Paket Wisata Ketapang</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>A0004</t>
+          <t>A0002</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-11-25 18:05:21.359478+07:00</t>
+          <t>2024-11-27 03:29:58.357326+07:00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>user2@gmail.com</t>
+          <t>rio@gmail.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>KSR_01</t>
+          <t>ADM_01</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -624,12 +628,12 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2024-11-25</t>
+          <t>2024-11-30</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2024-11-26</t>
+          <t>2024-12-01</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -651,7 +655,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-11-25 18:03:54.803392+07:00</t>
+          <t>2024-11-27 13:48:07.439755+07:00</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -661,7 +665,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>KSR_01</t>
+          <t>ADM_01</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -671,7 +675,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2280000.0</t>
+          <t>500000.0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -681,12 +685,12 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2024-11-25</t>
+          <t>2024-11-30</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2024-11-28</t>
+          <t>2024-12-01</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -694,7 +698,11 @@
           <t>PTKSKW</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Paket Wisata Singkawang</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -704,54 +712,103 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-11-25 18:05:21.359478+07:00</t>
+          <t>2024-11-27 13:50:28.081021+07:00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>user2@gmail.com</t>
+          <t>rio@gmail.com</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
+          <t>ADM_01</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>5220000.0</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>2024-11-27</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2024-11-29</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>PTKSKW</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>A0005</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2024-11-27 13:51:53.647278+07:00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>rio@gmail.com</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>KSR_01</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>COMPLETED</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>500000.0</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>cash</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>2024-11-30</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>2024-12-01</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>PTKSKW</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Paket Wisata Singkawang</t>
-        </is>
-      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>8400000.0</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>transfer</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>2024-11-28</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2024-11-29</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>KTPPTK</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Code Terakhir sebelum ubah websocket
</commit_message>
<xml_diff>
--- a/datapenjualan_bushub.xlsx
+++ b/datapenjualan_bushub.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -550,22 +550,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>A0002</t>
+          <t>A0001</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-11-28 22:20:39.659228+07:00</t>
+          <t>2025-01-20 22:03:57.412973+07:00</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>user2@gmail.com</t>
+          <t>ricardo@gmail.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>KSR_01</t>
+          <t>ADM_01</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -575,37 +575,37 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2520000.0</t>
+          <t>760000.0</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>cash</t>
+          <t>transfer</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2600000.0</t>
+          <t>760000.0</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>80000.0</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>2024-11-28</t>
+          <t>2025-01-20</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2024-11-28</t>
+          <t>2025-01-20</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>PTKKTP</t>
+          <t>PTKSKW</t>
         </is>
       </c>
       <c r="M5" t="inlineStr"/>
@@ -613,67 +613,130 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>A0001</t>
+          <t>A0002</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-11-28 22:20:08.224579+07:00</t>
+          <t>2025-01-20 22:13:39.509377+07:00</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>user2@gmail.com</t>
+          <t>user1@gmail.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>KSR_01</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2280000.0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>transfer</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2280000.0</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>2025-01-20</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2025-01-22</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>PTKSKW</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>A0003</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-01-20 22:15:12.821899+07:00</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>user1@gmail.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>ADM_01</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>COMPLETED</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>500000.0</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>transfer</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>500000.0</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>2024-11-30</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>2024-12-01</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>1500000.0</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>cash</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>1600000.0</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>100000.0</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2025-02-02</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2025-02-04</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
         <is>
           <t>PTKSKW</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>Paket Wisata Singkawang</t>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Paket Wisata Ketapang</t>
         </is>
       </c>
     </row>

</xml_diff>